<commit_message>
Added summary table and scripts for updated dataset
</commit_message>
<xml_diff>
--- a/data/LASI Family Variable List.xlsx
+++ b/data/LASI Family Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3FFCA6-1D1F-4744-994A-CFD0A73C19C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55EB6B6-11D4-4F93-826E-EF87D91C61E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -971,8 +971,8 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29:E34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1018,15 +1018,6 @@
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -1037,6 +1028,15 @@
       </c>
       <c r="C3" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1920,7 +1920,7 @@
       <c r="D81" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D82:D1048576 E17:F17 D1:D28 E29:E34 D38:D45 E35:F37 D47:D80 E52:F53 E55:F57">
+  <conditionalFormatting sqref="D82:D1048576 E17:F17 D3:D28 D1 E29:E34 D38:D45 E35:F37 D47:D80 E52:F53 E55:F57">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
@@ -1929,20 +1929,20 @@
   <conditionalFormatting sqref="B89:B1048576 B1:B14 B73:B84 B16:B60">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E11:E15">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F6">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F12 F18:F20 F15 G18">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E6">
+    <cfRule type="duplicateValues" dxfId="1" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F6">
+    <cfRule type="duplicateValues" dxfId="0" priority="26"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added analytic sample criteria as per Lee 2022
</commit_message>
<xml_diff>
--- a/data/LASI Family Variable List.xlsx
+++ b/data/LASI Family Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55EB6B6-11D4-4F93-826E-EF87D91C61E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2C8B2F-C89C-4273-8050-FC472EAF4E6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>hhid</t>
   </si>
   <si>
-    <t>education</t>
-  </si>
-  <si>
     <t>Number of children</t>
   </si>
   <si>
@@ -557,6 +554,9 @@
   </si>
   <si>
     <t>bm015</t>
+  </si>
+  <si>
+    <t>edulevel</t>
   </si>
 </sst>
 </file>
@@ -971,8 +971,8 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3:F3"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -987,33 +987,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
@@ -1021,50 +1021,50 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -1081,63 +1081,63 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -1145,10 +1145,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>12</v>
@@ -1165,65 +1165,65 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1231,647 +1231,647 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="D20" s="3"/>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" t="s">
         <v>130</v>
-      </c>
-      <c r="G25" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="C41" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E53" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="E57" t="s">
         <v>156</v>
-      </c>
-      <c r="E57" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>